<commit_message>
implement regulatory gene json loading
</commit_message>
<xml_diff>
--- a/CellWar.Document/game_data.xlsx
+++ b/CellWar.Document/game_data.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21727"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\iGEM-game\CellWar.Document\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{731AEB97-A92C-4602-8561-14393647296E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="28695" windowHeight="13200"/>
   </bookViews>
   <sheets>
     <sheet name="Regulatory" sheetId="1" r:id="rId1"/>
@@ -23,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89">
   <si>
     <t>Name</t>
   </si>
@@ -34,6 +28,9 @@
     <t>Chemical</t>
   </si>
   <si>
+    <t>Count</t>
+  </si>
+  <si>
     <t>Type</t>
   </si>
   <si>
@@ -49,7 +46,10 @@
     <t>Ampicillin</t>
   </si>
   <si>
-    <t>NegativeOrRegulartoryGene</t>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>假如Ampcilin抗生素数量大于50，基因关闭</t>
   </si>
   <si>
     <t>C2</t>
@@ -58,7 +58,10 @@
     <t>lactose</t>
   </si>
   <si>
-    <t>PositiveAllRegulatoryGene</t>
+    <t>PA</t>
+  </si>
+  <si>
+    <t>假如lactose抗生素数量大于100，基因打开</t>
   </si>
   <si>
     <t>与门</t>
@@ -70,7 +73,7 @@
     <t>IPTG</t>
   </si>
   <si>
-    <t>NegativeAllRegulartoryGene</t>
+    <t>假如IPTG抗生素数量大于100，基因打开</t>
   </si>
   <si>
     <t>非与门</t>
@@ -79,13 +82,22 @@
     <t>C4</t>
   </si>
   <si>
-    <t>PositiveOrRegulartoryGene</t>
+    <t>默认打开</t>
+  </si>
+  <si>
+    <t>PO</t>
   </si>
   <si>
     <t>或门</t>
   </si>
   <si>
     <t>RedLight</t>
+  </si>
+  <si>
+    <t>假如Ampcilin抗生素数量大于54，基因关闭</t>
+  </si>
+  <si>
+    <t>NO</t>
   </si>
   <si>
     <t>非或门</t>
@@ -372,9 +384,6 @@
     <t>Detailed</t>
   </si>
   <si>
-    <t>Count</t>
-  </si>
-  <si>
     <t>SpreadRate</t>
   </si>
   <si>
@@ -400,53 +409,22 @@
   </si>
   <si>
     <t>红光</t>
-  </si>
-  <si>
-    <t>Count</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>假如Ampcilin抗生素数量大于50，基因关闭</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>假如Ampcilin抗生素数量大于54，基因关闭</t>
-  </si>
-  <si>
-    <t>默认打开</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>假如IPTG抗生素数量大于100，基因打开</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>假如lactose抗生素数量大于100，基因打开</t>
-    <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+  </numFmts>
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -465,7 +443,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -474,27 +453,342 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
-      <family val="3"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="等线"/>
-      <family val="3"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -551,36 +845,321 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -838,28 +1417,28 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:J44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
-    <col min="5" max="5" width="25.6640625" customWidth="1"/>
-    <col min="6" max="6" width="38.5546875" customWidth="1"/>
-    <col min="7" max="7" width="12.88671875" customWidth="1"/>
-    <col min="9" max="9" width="25.21875" customWidth="1"/>
-    <col min="10" max="10" width="23.109375" customWidth="1"/>
+    <col min="5" max="5" width="25.6666666666667" customWidth="1"/>
+    <col min="6" max="6" width="38.5583333333333" customWidth="1"/>
+    <col min="7" max="7" width="12.8833333333333" customWidth="1"/>
+    <col min="9" max="9" width="25.2166666666667" customWidth="1"/>
+    <col min="10" max="10" width="23.1083333333333" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -870,93 +1449,93 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>84</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" s="2">
         <v>50</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D3" s="2">
         <v>100</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>89</v>
+        <v>13</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>14</v>
       </c>
       <c r="I3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="J3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D4" s="2">
         <v>100</v>
       </c>
       <c r="E4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>88</v>
+        <v>13</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>18</v>
       </c>
       <c r="I4" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="J4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -966,215 +1545,207 @@
         <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="12" t="s">
-        <v>87</v>
+        <v>13</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>21</v>
       </c>
       <c r="I5" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="J5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B6">
         <v>0</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D6" s="2">
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>86</v>
+        <v>9</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>25</v>
       </c>
       <c r="I6" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="J6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="3:4">
       <c r="C7" s="3"/>
       <c r="D7" s="2"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:4">
       <c r="C8" s="3"/>
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:4">
       <c r="C9" s="3"/>
       <c r="D9" s="2"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:4">
       <c r="C10" s="3"/>
       <c r="D10" s="2"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:4">
       <c r="C11" s="3"/>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:4">
       <c r="C12" s="3"/>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:4">
       <c r="C13" s="3"/>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:4">
       <c r="C14" s="3"/>
       <c r="D14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:4">
       <c r="C15" s="3"/>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:4">
       <c r="C16" s="3"/>
       <c r="D16" s="2"/>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:4">
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:4">
       <c r="D18" s="2"/>
     </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:4">
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:4">
       <c r="D20" s="2"/>
     </row>
-    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:4">
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:4">
       <c r="D22" s="2"/>
     </row>
-    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:4">
       <c r="D23" s="2"/>
     </row>
-    <row r="24" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:4">
       <c r="D24" s="2"/>
     </row>
-    <row r="25" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:4">
       <c r="D25" s="2"/>
     </row>
-    <row r="26" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:4">
       <c r="D26" s="2"/>
     </row>
-    <row r="27" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:4">
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:4">
       <c r="D28" s="2"/>
     </row>
-    <row r="29" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:4">
       <c r="D29" s="2"/>
     </row>
-    <row r="30" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:4">
       <c r="D30" s="2"/>
     </row>
-    <row r="31" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:4">
       <c r="D31" s="2"/>
     </row>
-    <row r="32" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:4">
       <c r="D32" s="2"/>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:4">
       <c r="D33" s="2"/>
     </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:4">
       <c r="D34" s="2"/>
     </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:4">
       <c r="D35" s="2"/>
     </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:4">
       <c r="D36" s="2"/>
     </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:4">
       <c r="D37" s="2"/>
     </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:4">
       <c r="D38" s="2"/>
     </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:4">
       <c r="D39" s="2"/>
     </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:4">
       <c r="D40" s="2"/>
     </row>
-    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:4">
       <c r="D41" s="2"/>
     </row>
-    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="4:4">
       <c r="D42" s="2"/>
     </row>
-    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="4:4">
       <c r="D43" s="2"/>
     </row>
-    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="4:4">
       <c r="D44" s="2"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E16" xr:uid="{00000000-0002-0000-0000-000001000000}">
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C16">
+      <formula1>Chemical!$A:$A</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E16">
       <formula1>$I$3:$I$6</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
-          <x14:formula1>
-            <xm:f>Chemical!$A:$A</xm:f>
-          </x14:formula1>
-          <xm:sqref>C2:C16</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:M55"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="12.21875" customWidth="1"/>
-    <col min="3" max="3" width="54.77734375" customWidth="1"/>
-    <col min="4" max="5" width="19.77734375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="25.88671875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="12.2166666666667" customWidth="1"/>
+    <col min="3" max="3" width="54.775" customWidth="1"/>
+    <col min="4" max="5" width="19.775" style="2" customWidth="1"/>
+    <col min="6" max="6" width="25.8833333333333" style="3" customWidth="1"/>
     <col min="7" max="8" width="29" style="2" customWidth="1"/>
-    <col min="9" max="9" width="21.33203125" style="3" customWidth="1"/>
-    <col min="10" max="10" width="25.33203125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="26.33203125" style="4" customWidth="1"/>
-    <col min="12" max="12" width="19.44140625" customWidth="1"/>
-    <col min="13" max="13" width="19.109375" customWidth="1"/>
+    <col min="9" max="9" width="21.3333333333333" style="3" customWidth="1"/>
+    <col min="10" max="10" width="25.3333333333333" style="2" customWidth="1"/>
+    <col min="11" max="11" width="26.3333333333333" style="4" customWidth="1"/>
+    <col min="12" max="12" width="19.4416666666667" customWidth="1"/>
+    <col min="13" max="13" width="19.1083333333333" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1182,48 +1753,48 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="K1" s="11" t="s">
-        <v>30</v>
+        <v>35</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>36</v>
       </c>
       <c r="L1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="M1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" s="8" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="D2" s="2">
         <v>0.1</v>
@@ -1238,7 +1809,7 @@
         <v>0</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="J2" s="2">
         <v>0.1</v>
@@ -1253,15 +1824,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
-        <v>36</v>
+    <row r="3" spans="1:13">
+      <c r="A3" s="8" t="s">
+        <v>42</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="D3" s="2">
         <v>0.3</v>
@@ -1276,7 +1847,7 @@
         <v>0</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="J3" s="2">
         <v>0.5</v>
@@ -1291,15 +1862,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13">
       <c r="A4" s="8" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="D4" s="2">
         <v>0.9</v>
@@ -1314,7 +1885,7 @@
         <v>0</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="J4" s="2">
         <v>0.8</v>
@@ -1329,15 +1900,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
-        <v>40</v>
+    <row r="5" spans="1:13">
+      <c r="A5" s="8" t="s">
+        <v>46</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="D5" s="2">
         <v>1</v>
@@ -1352,7 +1923,7 @@
         <v>0</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="J5" s="2">
         <v>0.1</v>
@@ -1367,15 +1938,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13">
       <c r="A6" s="8" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="B6">
         <v>0</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="D6" s="2">
         <v>0.1</v>
@@ -1390,7 +1961,7 @@
         <v>0</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="J6" s="2">
         <v>0.1</v>
@@ -1405,15 +1976,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
-        <v>44</v>
+    <row r="7" spans="1:13">
+      <c r="A7" s="8" t="s">
+        <v>50</v>
       </c>
       <c r="B7">
         <v>0</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="D7" s="2">
         <v>0</v>
@@ -1428,7 +1999,7 @@
         <v>0</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="J7" s="2">
         <v>0.1</v>
@@ -1443,15 +2014,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13">
       <c r="A8" s="8" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="B8">
         <v>0</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="D8" s="2">
         <v>0</v>
@@ -1466,7 +2037,7 @@
         <v>0</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="J8" s="2">
         <v>0.1</v>
@@ -1481,15 +2052,15 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
-        <v>47</v>
+    <row r="9" spans="1:13">
+      <c r="A9" s="8" t="s">
+        <v>53</v>
       </c>
       <c r="B9">
         <v>0</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="D9" s="2">
         <v>0</v>
@@ -1504,7 +2075,7 @@
         <v>0</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="J9" s="2">
         <v>0.1</v>
@@ -1519,15 +2090,15 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
-        <v>49</v>
+    <row r="10" spans="1:13">
+      <c r="A10" s="8" t="s">
+        <v>55</v>
       </c>
       <c r="B10">
         <v>0</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="D10" s="2">
         <v>0</v>
@@ -1542,7 +2113,7 @@
         <v>0</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="J10" s="2">
         <v>0.1</v>
@@ -1557,15 +2128,15 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13">
       <c r="A11" s="8" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="B11">
         <v>0</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="D11" s="2">
         <v>-0.2</v>
@@ -1592,15 +2163,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
-        <v>53</v>
+    <row r="12" spans="1:13">
+      <c r="A12" s="8" t="s">
+        <v>59</v>
       </c>
       <c r="B12">
         <v>0</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="D12" s="2">
         <v>-0.5</v>
@@ -1627,15 +2198,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
-        <v>53</v>
+    <row r="13" spans="1:13">
+      <c r="A13" s="8" t="s">
+        <v>59</v>
       </c>
       <c r="B13">
         <v>0</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="D13" s="2">
         <v>-1</v>
@@ -1650,7 +2221,7 @@
         <v>0</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="J13" s="2">
         <v>0.1</v>
@@ -1665,15 +2236,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13">
       <c r="A14" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="B14">
         <v>554</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="D14" s="2">
         <v>0</v>
@@ -1700,15 +2271,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13">
       <c r="A15" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="B15">
         <v>516</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="D15" s="2">
         <v>0</v>
@@ -1717,7 +2288,7 @@
         <v>0</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="G15" s="6">
         <v>0.1</v>
@@ -1738,15 +2309,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13">
       <c r="A16" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="B16">
         <v>643</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="D16" s="2">
         <v>0</v>
@@ -1755,7 +2326,7 @@
         <v>0</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="G16" s="6">
         <v>0.1</v>
@@ -1776,15 +2347,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13">
       <c r="A17" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="B17">
         <v>345</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="D17" s="2">
         <v>0</v>
@@ -1799,7 +2370,7 @@
         <v>0</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="J17" s="2">
         <v>0.1</v>
@@ -1814,15 +2385,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13">
       <c r="A18" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="B18">
         <v>345</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="D18" s="2">
         <v>0</v>
@@ -1837,7 +2408,7 @@
         <v>0</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="J18" s="2">
         <v>0.1</v>
@@ -1852,15 +2423,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13">
       <c r="A19" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="B19">
         <v>0</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="D19" s="2">
         <v>0</v>
@@ -1875,7 +2446,7 @@
         <v>0</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J19" s="2">
         <v>0.1</v>
@@ -1890,15 +2461,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="10" t="s">
-        <v>68</v>
+    <row r="20" spans="1:13">
+      <c r="A20" s="9" t="s">
+        <v>74</v>
       </c>
       <c r="B20">
         <v>0</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="D20" s="2">
         <v>0</v>
@@ -1907,7 +2478,7 @@
         <v>0</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="G20" s="6">
         <v>0.1</v>
@@ -1916,7 +2487,7 @@
         <v>0</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="J20" s="2">
         <v>0.1</v>
@@ -1931,15 +2502,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
-        <v>71</v>
+    <row r="21" spans="1:13">
+      <c r="A21" s="8" t="s">
+        <v>77</v>
       </c>
       <c r="B21">
         <v>0</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="D21" s="2">
         <v>0</v>
@@ -1948,7 +2519,7 @@
         <v>0</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="G21" s="6">
         <v>1</v>
@@ -1969,7 +2540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:13">
       <c r="B22">
         <v>0</v>
       </c>
@@ -1998,7 +2569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:13">
       <c r="B23">
         <v>0</v>
       </c>
@@ -2027,7 +2598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:13">
       <c r="B24">
         <v>0</v>
       </c>
@@ -2056,7 +2627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:13">
       <c r="B25">
         <v>0</v>
       </c>
@@ -2085,7 +2656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:13">
       <c r="B26">
         <v>0</v>
       </c>
@@ -2114,7 +2685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:13">
       <c r="B27">
         <v>0</v>
       </c>
@@ -2143,7 +2714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:13">
       <c r="B28">
         <v>0</v>
       </c>
@@ -2172,7 +2743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:13">
       <c r="B29">
         <v>0</v>
       </c>
@@ -2201,7 +2772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:13">
       <c r="B30">
         <v>0</v>
       </c>
@@ -2230,7 +2801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:13">
       <c r="B31">
         <v>0</v>
       </c>
@@ -2256,7 +2827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:13">
       <c r="B32">
         <v>0</v>
       </c>
@@ -2282,7 +2853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:13">
       <c r="B33">
         <v>0</v>
       </c>
@@ -2308,7 +2879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:13">
       <c r="B34">
         <v>0</v>
       </c>
@@ -2334,7 +2905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:13">
       <c r="B35">
         <v>0</v>
       </c>
@@ -2360,7 +2931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:13">
       <c r="B36">
         <v>0</v>
       </c>
@@ -2386,7 +2957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:13">
       <c r="B37">
         <v>0</v>
       </c>
@@ -2412,7 +2983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:13">
       <c r="B38">
         <v>0</v>
       </c>
@@ -2438,7 +3009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:13">
       <c r="B39">
         <v>0</v>
       </c>
@@ -2464,7 +3035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="7:13">
       <c r="G40" s="6">
         <v>0</v>
       </c>
@@ -2484,7 +3055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="7:13">
       <c r="G41" s="6">
         <v>0</v>
       </c>
@@ -2504,7 +3075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="7:13">
       <c r="G42" s="6">
         <v>0</v>
       </c>
@@ -2524,7 +3095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="7:13">
       <c r="G43" s="6">
         <v>0</v>
       </c>
@@ -2544,7 +3115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="7:13">
       <c r="G44" s="6">
         <v>0</v>
       </c>
@@ -2564,7 +3135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="7:13">
       <c r="G45" s="6">
         <v>0</v>
       </c>
@@ -2584,7 +3155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="7:13">
       <c r="G46" s="6">
         <v>0</v>
       </c>
@@ -2604,7 +3175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="7:13">
       <c r="G47" s="6">
         <v>0</v>
       </c>
@@ -2624,7 +3195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="7:13">
       <c r="G48" s="6">
         <v>0</v>
       </c>
@@ -2644,7 +3215,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="7:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="7:13">
       <c r="G49" s="6">
         <v>0</v>
       </c>
@@ -2664,7 +3235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="7:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="7:13">
       <c r="G50" s="6">
         <v>0</v>
       </c>
@@ -2684,7 +3255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="7:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="7:13">
       <c r="G51" s="6">
         <v>0</v>
       </c>
@@ -2704,7 +3275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="7:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="7:13">
       <c r="G52" s="6">
         <v>0</v>
       </c>
@@ -2724,7 +3295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="7:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="7:13">
       <c r="G53" s="6">
         <v>0</v>
       </c>
@@ -2744,7 +3315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="7:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="7:13">
       <c r="G54" s="6">
         <v>0</v>
       </c>
@@ -2764,7 +3335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="7:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="7:13">
       <c r="G55" s="6">
         <v>0</v>
       </c>
@@ -2785,146 +3356,143 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="7" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F39 I2:I39">
+      <formula1>Chemical!$A:$A</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
-          <x14:formula1>
-            <xm:f>Chemical!$A:$A</xm:f>
-          </x14:formula1>
-          <xm:sqref>F2:F39 I2:I39</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="32.44140625" customWidth="1"/>
+    <col min="1" max="1" width="32.4416666666667" customWidth="1"/>
     <col min="2" max="2" width="74" customWidth="1"/>
-    <col min="5" max="5" width="17.88671875" customWidth="1"/>
+    <col min="5" max="5" width="17.8833333333333" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="D1" t="s">
-        <v>74</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>71</v>
-      </c>
-      <c r="B5" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="B8" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="B9" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2">
       <c r="B11" s="1"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="7" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <sheetData/>
-  <phoneticPr fontId="7" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>